<commit_message>
Added all data processed to python. Next step is to plot and write further notes
</commit_message>
<xml_diff>
--- a/systematic_data_analysis.xlsx
+++ b/systematic_data_analysis.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="155">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,414 @@
   </si>
   <si>
     <t>F1F7_B9_H</t>
+  </si>
+  <si>
+    <t>F9F10_B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get stuck some times </t>
+  </si>
+  <si>
+    <t>got stuck at the end, not super consistent</t>
+  </si>
+  <si>
+    <t>go stuck, but was working alright, not shorted</t>
+  </si>
+  <si>
+    <t>F8F15_B1_b_</t>
+  </si>
+  <si>
+    <t>quit because ... (this is a test)</t>
+  </si>
+  <si>
+    <t>F8F15_B1_A_withdrop</t>
+  </si>
+  <si>
+    <t>no shorting up to 80 V, wet, probe station hood open</t>
+  </si>
+  <si>
+    <t>did not short with drop of DI water</t>
+  </si>
+  <si>
+    <t>F8F15_B1_A_</t>
+  </si>
+  <si>
+    <t>F8F15_B2_F_meas2</t>
+  </si>
+  <si>
+    <t>shorted at some poin, use later data for resistance computing</t>
+  </si>
+  <si>
+    <t>F8F15_B4_e_meas2</t>
+  </si>
+  <si>
+    <t>32 ms is wrong, stopped moving</t>
+  </si>
+  <si>
+    <t>clunky</t>
+  </si>
+  <si>
+    <t>F8F15_B2_H_meas3</t>
+  </si>
+  <si>
+    <t>did not move anymoe</t>
+  </si>
+  <si>
+    <t>F8F15_B2_H_meas2</t>
+  </si>
+  <si>
+    <t>note that the actual voltage does not reflect power supply, dev works</t>
+  </si>
+  <si>
+    <t>F8F15_B2_G_meas2</t>
+  </si>
+  <si>
+    <t>shorted, but data is useful to estimate resistance of short</t>
+  </si>
+  <si>
+    <t>weird struggle at small voltages</t>
+  </si>
+  <si>
+    <t>F8F15_B2_D_meas3</t>
+  </si>
+  <si>
+    <t>reapeat same with flipped driving electrodes</t>
+  </si>
+  <si>
+    <t>F8F15_B2_D_meas2</t>
+  </si>
+  <si>
+    <t>stopped workin at some point</t>
+  </si>
+  <si>
+    <t>moves back and forth, continue to higher v</t>
+  </si>
+  <si>
+    <t>back and forth motion at 60 hz</t>
+  </si>
+  <si>
+    <t>F8F15_B2_C_meas2</t>
+  </si>
+  <si>
+    <t>needs higher voltage</t>
+  </si>
+  <si>
+    <t>interrupted by mistake, good data</t>
+  </si>
+  <si>
+    <t>F8F15_B2_B_meas2</t>
+  </si>
+  <si>
+    <t>shorted after going above 100 V, note the resistance once shorted. Might be issue with probe</t>
+  </si>
+  <si>
+    <t>was stuck at low voltages, raised it to get unstuck</t>
+  </si>
+  <si>
+    <t>F8F15_B2_A_meas2</t>
+  </si>
+  <si>
+    <t>shorted</t>
+  </si>
+  <si>
+    <t>F8F15_B6_B_meas2</t>
+  </si>
+  <si>
+    <t>stopped woking when doing 45V, 64 ms. Seems stuck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no field of name trigger_signal2 </t>
+  </si>
+  <si>
+    <t>F7_NB10_G_south</t>
+  </si>
+  <si>
+    <t>did not see motion. Measuring east west current spikes</t>
+  </si>
+  <si>
+    <t>F8F15_B7_A_meas2</t>
+  </si>
+  <si>
+    <t>clunky but works (weird since serpentine springs are broken)</t>
+  </si>
+  <si>
+    <t>object got stuck, maybe electrical data shows why?</t>
+  </si>
+  <si>
+    <t>F8F15_B7_B_meas2</t>
+  </si>
+  <si>
+    <t>got stuck, compare to previous measurements</t>
+  </si>
+  <si>
+    <t>works ok. definitely worth plotting. Note that 35 and 50 V for 4ms are flipped (mistake in acquisition)</t>
+  </si>
+  <si>
+    <t>F8F15_B8_C_meas2</t>
+  </si>
+  <si>
+    <t>interupted by eror, works more or less, continued in next ecording</t>
+  </si>
+  <si>
+    <t>F8F15_B9_A_meas2</t>
+  </si>
+  <si>
+    <t>broke after few things</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal3</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal4</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal5</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal6</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal7</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal8</t>
+  </si>
+  <si>
+    <t>no field of name trigger_signal9</t>
+  </si>
+  <si>
+    <t>F7_NB11_C_meas2</t>
+  </si>
+  <si>
+    <t>gets stuck and then unstuck, but East and West still stuck. Image depics South gca but triggered for east west</t>
+  </si>
+  <si>
+    <t>driver error, input voltage not useful</t>
+  </si>
+  <si>
+    <t>stopped working, but other side was woking</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr1c1_meas2</t>
+  </si>
+  <si>
+    <t>useful data</t>
+  </si>
+  <si>
+    <t>good data, pull in 43.75</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr1c2_meas2</t>
+  </si>
+  <si>
+    <t>stuck, physically broken? No pull in measured</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr1c3_meas2</t>
+  </si>
+  <si>
+    <t>pull in 14.18 (first time measured was much higher), good data</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr2c1_meas2</t>
+  </si>
+  <si>
+    <t>stuck, no pull in. The issu comes from unsucessful bonding?</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr2c2_meas2</t>
+  </si>
+  <si>
+    <t>pull in 29.25 V, worked well up to a poin, then something stuck? prevents full pull in</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr3c1_meas2</t>
+  </si>
+  <si>
+    <t>pull in 30.75 V. Useful data</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr3c2_meas2</t>
+  </si>
+  <si>
+    <t>driver eror, retake all data. Good. Pull in 26.0V</t>
+  </si>
+  <si>
+    <t>26.0 V pull in, good data</t>
+  </si>
+  <si>
+    <t>F7_NB11_Pr3c3_meas2</t>
+  </si>
+  <si>
+    <t>stuck after a certain amount. Be carefuly with current data (might be off) PIV 13.75</t>
+  </si>
+  <si>
+    <t>F8F15_B15_B_meas2</t>
+  </si>
+  <si>
+    <t>able to see pull in, moved some at 40 V but got stuck</t>
+  </si>
+  <si>
+    <t>can tell pull in? is stuck. Will redo hole range with shorter read windows</t>
+  </si>
+  <si>
+    <t>electrical data for all of it, is it stuck now</t>
+  </si>
+  <si>
+    <t>see leackage current at higher values</t>
+  </si>
+  <si>
+    <t>F8F15_B15_C_meas2</t>
+  </si>
+  <si>
+    <t>no motion, no shorting, go higher voltage</t>
+  </si>
+  <si>
+    <t>fingers bending? seems stuck. Will try probe to push out and then restart</t>
+  </si>
+  <si>
+    <t>F8F15_B15_E_meas2</t>
+  </si>
+  <si>
+    <t>driver error, save progress so far</t>
+  </si>
+  <si>
+    <t>shorted, good way to show when one electrode is shorted to ground, get maginuted of short (total resistance)</t>
+  </si>
+  <si>
+    <t>F8F15_B15_F_meas2</t>
+  </si>
+  <si>
+    <t>example of other electrode shorted from get go</t>
+  </si>
+  <si>
+    <t>F8F15_B15_G_meas2</t>
+  </si>
+  <si>
+    <t>shorted around 40 V input, see current data</t>
+  </si>
+  <si>
+    <t>F8F15_B15_H_meas2</t>
+  </si>
+  <si>
+    <t>one electrode shorted after going to 30 V</t>
+  </si>
+  <si>
+    <t>F8F15_B1A_B_dr</t>
+  </si>
+  <si>
+    <t>dry, will change to wet to compare electrical data</t>
+  </si>
+  <si>
+    <t>F8F15_B1A_B_wet_nothydrophobicforsomereason</t>
+  </si>
+  <si>
+    <t>wet, note that electrolysis was occuring, see videos for bubbles</t>
+  </si>
+  <si>
+    <t>F8F15_B1A_D_meas2</t>
+  </si>
+  <si>
+    <t>shorted at around 60V, but could be usefull for force computations?</t>
+  </si>
+  <si>
+    <t>F8F15_B14_rotA_meas2</t>
+  </si>
+  <si>
+    <t>shorted at 40V, example with old designs</t>
+  </si>
+  <si>
+    <t>F8F15_B15_A_meas2</t>
+  </si>
+  <si>
+    <t>some motion at 40, but got stuck</t>
+  </si>
+  <si>
+    <t>F8F15_B17_A_dry</t>
+  </si>
+  <si>
+    <t>may have some usefull data but will remeasure</t>
+  </si>
+  <si>
+    <t>dry conditions, will performe same test with drop</t>
+  </si>
+  <si>
+    <t>F8F15_B17_H_dry</t>
+  </si>
+  <si>
+    <t>did not move. Sometimes it shorts but then it goes away, not sure whats up</t>
+  </si>
+  <si>
+    <t>F8F15_B18_C_P1P2 not P3 wet</t>
+  </si>
+  <si>
+    <t>wet, does not move but is not shorted, might be missing data (driver error</t>
+  </si>
+  <si>
+    <t>does not move, scale up voltage</t>
+  </si>
+  <si>
+    <t>F8F15_B18_C_P1P2 not P3</t>
+  </si>
+  <si>
+    <t>single set of pawls works well</t>
+  </si>
+  <si>
+    <t>F8F15_B18_g_only two pawls</t>
+  </si>
+  <si>
+    <t>works okay with a single set of pawls, dry. Only the first and second pads are connected</t>
+  </si>
+  <si>
+    <t>F8F15_B18_g_only two pawls wet</t>
+  </si>
+  <si>
+    <t>does not moved, failed :(</t>
+  </si>
+  <si>
+    <t>a lot more noise, try higher voltages</t>
+  </si>
+  <si>
+    <t>F8F15_B18_E_P1P2P3</t>
+  </si>
+  <si>
+    <t>wet, isn't shorted, does not move at all. Previous meas was also wet. Could it be that it moves a bit and then surface forces dominate</t>
+  </si>
+  <si>
+    <t>moved a litle before recording</t>
+  </si>
+  <si>
+    <t>counter clockwise rotation</t>
+  </si>
+  <si>
+    <t>struggles but moves, other electrode shorted so disconnected</t>
+  </si>
+  <si>
+    <t>F8F15_B18_E_P1P2_only</t>
+  </si>
+  <si>
+    <t>single one, across voltages. Sometimes runs in oposite direction</t>
+  </si>
+  <si>
+    <t>F8F15_B18_C_P1P2P3 wet</t>
+  </si>
+  <si>
+    <t>both electrodes, no shorting under water, does no move</t>
+  </si>
+  <si>
+    <t>works well really fast frequencies</t>
+  </si>
+  <si>
+    <t>pushing speed limits, works decently</t>
+  </si>
+  <si>
+    <t>works very well, all frequencies, 60 V</t>
+  </si>
+  <si>
+    <t>runs well even at 1 ms</t>
+  </si>
+  <si>
+    <t>single electrode, failed at 8 ms</t>
   </si>
 </sst>
 </file>
@@ -399,16 +807,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="28.921875" customWidth="1"/>
-    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="2" max="2" width="43.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="13.3046875" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
   </cols>
@@ -557,6 +966,1170 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>20231002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>210671</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>20231002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>213817</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>20231008</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>170073</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>20231008</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>175635</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>20231008</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>174037</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>20231008</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>171634</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>20231010</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>165693</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>20231010</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>213629</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>20231010</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>213244</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>20231010</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>140553</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>20231010</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>135758</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>20231010</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>150144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>20231010</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>165693</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>20231010</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>164641</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>20231010</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <v>142699</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>20231010</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25">
+        <v>145028</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>20231010</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26">
+        <v>144282</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>20231010</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>143220</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>20231010</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>153402</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>20231010</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>151726</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>20231010</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>161038</v>
+      </c>
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>20231010</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31">
+        <v>145028</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>20231010</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>160526</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>20231010</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33">
+        <v>171198</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>20231011</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34">
+        <v>223670</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>20231012</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35">
+        <v>172730</v>
+      </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>20231012</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <v>152311</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>20231012</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>152859</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>20231012</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38">
+        <v>144913</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>20231012</v>
+      </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39">
+        <v>151076</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>20231012</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40">
+        <v>175671</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>20231012</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41">
+        <v>183592</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>20231017</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42">
+        <v>201391</v>
+      </c>
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>20231017</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43">
+        <v>202794</v>
+      </c>
+      <c r="E43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>20231017</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44">
+        <v>203240</v>
+      </c>
+      <c r="E44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>20231017</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45">
+        <v>210258</v>
+      </c>
+      <c r="E45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>20231017</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46">
+        <v>211209</v>
+      </c>
+      <c r="E46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>20231017</v>
+      </c>
+      <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47">
+        <v>212112</v>
+      </c>
+      <c r="E47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>20231017</v>
+      </c>
+      <c r="B48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48">
+        <v>213513</v>
+      </c>
+      <c r="E48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>20231017</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49">
+        <v>215105</v>
+      </c>
+      <c r="E49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>20231017</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50">
+        <v>220156</v>
+      </c>
+      <c r="E50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>20231017</v>
+      </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51">
+        <v>221860</v>
+      </c>
+      <c r="E51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>20231017</v>
+      </c>
+      <c r="B52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52">
+        <v>222700</v>
+      </c>
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>20231017</v>
+      </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53">
+        <v>223117</v>
+      </c>
+      <c r="E53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>20231017</v>
+      </c>
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54">
+        <v>223792</v>
+      </c>
+      <c r="E54" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>20231025</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55">
+        <v>222771</v>
+      </c>
+      <c r="E55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>20231025</v>
+      </c>
+      <c r="B56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56">
+        <v>223323</v>
+      </c>
+      <c r="E56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>20231025</v>
+      </c>
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57">
+        <v>225156</v>
+      </c>
+      <c r="E57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>20231025</v>
+      </c>
+      <c r="B58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58">
+        <v>233016</v>
+      </c>
+      <c r="E58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>20231025</v>
+      </c>
+      <c r="B59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59">
+        <v>220675</v>
+      </c>
+      <c r="E59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>20231025</v>
+      </c>
+      <c r="B60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60">
+        <v>221389</v>
+      </c>
+      <c r="E60" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>20231025</v>
+      </c>
+      <c r="B61" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61">
+        <v>233849</v>
+      </c>
+      <c r="E61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>20231025</v>
+      </c>
+      <c r="B62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62">
+        <v>234254</v>
+      </c>
+      <c r="E62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>20231025</v>
+      </c>
+      <c r="B63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63">
+        <v>235452</v>
+      </c>
+      <c r="E63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>20231025</v>
+      </c>
+      <c r="B64" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64">
+        <v>215416</v>
+      </c>
+      <c r="E64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>20231025</v>
+      </c>
+      <c r="B65" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65">
+        <v>213009</v>
+      </c>
+      <c r="E65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>20231026</v>
+      </c>
+      <c r="B66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66">
+        <v>4814</v>
+      </c>
+      <c r="E66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>20231026</v>
+      </c>
+      <c r="B67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67">
+        <v>10331</v>
+      </c>
+      <c r="E67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>20231026</v>
+      </c>
+      <c r="B68" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68">
+        <v>3736</v>
+      </c>
+      <c r="E68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>20231026</v>
+      </c>
+      <c r="B69" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69">
+        <v>1596</v>
+      </c>
+      <c r="E69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>20231026</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70">
+        <v>288</v>
+      </c>
+      <c r="E70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>20231027</v>
+      </c>
+      <c r="B71" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71">
+        <v>121530</v>
+      </c>
+      <c r="E71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>20231027</v>
+      </c>
+      <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72">
+        <v>122351</v>
+      </c>
+      <c r="E72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>20231027</v>
+      </c>
+      <c r="B73" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73">
+        <v>114313</v>
+      </c>
+      <c r="E73" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>20231028</v>
+      </c>
+      <c r="B74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74">
+        <v>210210</v>
+      </c>
+      <c r="E74" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>20231028</v>
+      </c>
+      <c r="B75" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75">
+        <v>210873</v>
+      </c>
+      <c r="E75" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>20231028</v>
+      </c>
+      <c r="B76" t="s">
+        <v>134</v>
+      </c>
+      <c r="C76">
+        <v>164859</v>
+      </c>
+      <c r="E76" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>20231028</v>
+      </c>
+      <c r="B77" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77">
+        <v>195519</v>
+      </c>
+      <c r="E77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>20231028</v>
+      </c>
+      <c r="B78" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78">
+        <v>200298</v>
+      </c>
+      <c r="E78" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>20231028</v>
+      </c>
+      <c r="B79" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79">
+        <v>200780</v>
+      </c>
+      <c r="E79" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>20231028</v>
+      </c>
+      <c r="B80" t="s">
+        <v>134</v>
+      </c>
+      <c r="C80">
+        <v>201690</v>
+      </c>
+      <c r="E80" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>20231028</v>
+      </c>
+      <c r="B81" t="s">
+        <v>134</v>
+      </c>
+      <c r="C81">
+        <v>202676</v>
+      </c>
+      <c r="E81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>20231028</v>
+      </c>
+      <c r="B82" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82">
+        <v>211455</v>
+      </c>
+      <c r="E82" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>20231028</v>
+      </c>
+      <c r="B83" t="s">
+        <v>146</v>
+      </c>
+      <c r="C83">
+        <v>212666</v>
+      </c>
+      <c r="E83" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>20231028</v>
+      </c>
+      <c r="B84" t="s">
+        <v>141</v>
+      </c>
+      <c r="C84">
+        <v>213039</v>
+      </c>
+      <c r="E84" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>20231028</v>
+      </c>
+      <c r="B85" t="s">
+        <v>141</v>
+      </c>
+      <c r="C85">
+        <v>213679</v>
+      </c>
+      <c r="E85" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>20231028</v>
+      </c>
+      <c r="B86" t="s">
+        <v>141</v>
+      </c>
+      <c r="C86">
+        <v>215754</v>
+      </c>
+      <c r="E86" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>20231028</v>
+      </c>
+      <c r="B87" t="s">
+        <v>141</v>
+      </c>
+      <c r="C87">
+        <v>220313</v>
+      </c>
+      <c r="E87" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>20231028</v>
+      </c>
+      <c r="B88" t="s">
+        <v>138</v>
+      </c>
+      <c r="C88">
+        <v>160169</v>
+      </c>
+      <c r="E88" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>20231028</v>
+      </c>
+      <c r="B89" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89">
+        <v>162771</v>
+      </c>
+      <c r="E89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>20231028</v>
+      </c>
+      <c r="B90" t="s">
+        <v>136</v>
+      </c>
+      <c r="C90">
+        <v>154643</v>
+      </c>
+      <c r="E90" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Lots of changes, should of edited sooner
</commit_message>
<xml_diff>
--- a/systematic_data_analysis.xlsx
+++ b/systematic_data_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15531" windowHeight="6549"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15533" windowHeight="6548"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="165">
   <si>
     <t>Date</t>
   </si>
@@ -490,6 +490,36 @@
   </si>
   <si>
     <t>single electrode, failed at 8 ms</t>
+  </si>
+  <si>
+    <t>Plotted. Steps take back and forth (small reduction of steps)</t>
+  </si>
+  <si>
+    <t>Analysis notes</t>
+  </si>
+  <si>
+    <t>No motion</t>
+  </si>
+  <si>
+    <t>Good videos, problem tracking F1F7_B9_B_4ms_40V</t>
+  </si>
+  <si>
+    <t>video out of focus, no motion. 16 ms/35 V shows some motion. 32 ms /35 v back and forth motion</t>
+  </si>
+  <si>
+    <t>Not very useful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good at 35 and 40 V </t>
+  </si>
+  <si>
+    <t>40 V nice clear steps</t>
+  </si>
+  <si>
+    <t>Useless</t>
+  </si>
+  <si>
+    <t>Clear videos for some voltages. See graphs</t>
   </si>
 </sst>
 </file>
@@ -807,22 +837,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.921875" customWidth="1"/>
-    <col min="2" max="2" width="43.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.9296875" customWidth="1"/>
+    <col min="2" max="2" width="43.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
+    <col min="6" max="6" width="20.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -838,8 +869,11 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>20230927</v>
       </c>
@@ -853,7 +887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>20230927</v>
       </c>
@@ -866,8 +900,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>20230927</v>
       </c>
@@ -880,8 +917,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>20230927</v>
       </c>
@@ -897,8 +937,11 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>20230927</v>
       </c>
@@ -914,8 +957,11 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>20230927</v>
       </c>
@@ -931,8 +977,11 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>20230927</v>
       </c>
@@ -948,8 +997,11 @@
       <c r="E8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>20230927</v>
       </c>
@@ -965,8 +1017,11 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>20231002</v>
       </c>
@@ -982,8 +1037,11 @@
       <c r="E10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>20231002</v>
       </c>
@@ -1000,7 +1058,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>20231008</v>
       </c>
@@ -1014,7 +1072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>20231008</v>
       </c>
@@ -1028,7 +1086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>20231008</v>
       </c>
@@ -1042,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>20231008</v>
       </c>
@@ -1056,7 +1114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>20231010</v>
       </c>
@@ -1070,7 +1128,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>20231010</v>
       </c>
@@ -1084,7 +1142,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>20231010</v>
       </c>
@@ -1098,7 +1156,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>20231010</v>
       </c>
@@ -1112,7 +1170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>20231010</v>
       </c>
@@ -1126,7 +1184,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20231010</v>
       </c>
@@ -1140,7 +1198,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20231010</v>
       </c>
@@ -1154,7 +1212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>20231010</v>
       </c>
@@ -1168,7 +1226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>20231010</v>
       </c>
@@ -1182,7 +1240,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>20231010</v>
       </c>
@@ -1196,7 +1254,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>20231010</v>
       </c>
@@ -1210,7 +1268,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>20231010</v>
       </c>
@@ -1224,7 +1282,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>20231010</v>
       </c>
@@ -1238,7 +1296,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>20231010</v>
       </c>
@@ -1252,7 +1310,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>20231010</v>
       </c>
@@ -1266,7 +1324,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>20231010</v>
       </c>
@@ -1280,7 +1338,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>20231010</v>
       </c>
@@ -1294,7 +1352,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>20231010</v>
       </c>
@@ -1308,7 +1366,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>20231011</v>
       </c>
@@ -1325,7 +1383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>20231012</v>
       </c>
@@ -1342,7 +1400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>20231012</v>
       </c>
@@ -1359,7 +1417,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>20231012</v>
       </c>
@@ -1376,7 +1434,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>20231012</v>
       </c>
@@ -1393,7 +1451,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>20231012</v>
       </c>
@@ -1410,7 +1468,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>20231012</v>
       </c>
@@ -1427,7 +1485,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>20231012</v>
       </c>
@@ -1444,7 +1502,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>20231017</v>
       </c>
@@ -1458,7 +1516,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>20231017</v>
       </c>
@@ -1472,7 +1530,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>20231017</v>
       </c>
@@ -1486,7 +1544,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>20231017</v>
       </c>
@@ -1500,7 +1558,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>20231017</v>
       </c>
@@ -1514,7 +1572,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>20231017</v>
       </c>
@@ -1528,7 +1586,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>20231017</v>
       </c>
@@ -1542,7 +1600,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>20231017</v>
       </c>
@@ -1556,7 +1614,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>20231017</v>
       </c>
@@ -1570,7 +1628,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>20231017</v>
       </c>
@@ -1584,7 +1642,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>20231017</v>
       </c>
@@ -1598,7 +1656,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>20231017</v>
       </c>
@@ -1612,7 +1670,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>20231017</v>
       </c>
@@ -1626,7 +1684,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>20231025</v>
       </c>
@@ -1640,7 +1698,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>20231025</v>
       </c>
@@ -1654,7 +1712,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>20231025</v>
       </c>
@@ -1668,7 +1726,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>20231025</v>
       </c>
@@ -1682,7 +1740,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>20231025</v>
       </c>
@@ -1696,7 +1754,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>20231025</v>
       </c>
@@ -1710,7 +1768,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>20231025</v>
       </c>
@@ -1724,7 +1782,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>20231025</v>
       </c>
@@ -1738,7 +1796,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>20231025</v>
       </c>
@@ -1752,7 +1810,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>20231025</v>
       </c>
@@ -1766,7 +1824,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>20231025</v>
       </c>
@@ -1780,7 +1838,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>20231026</v>
       </c>
@@ -1794,7 +1852,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>20231026</v>
       </c>
@@ -1808,7 +1866,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>20231026</v>
       </c>
@@ -1822,7 +1880,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>20231026</v>
       </c>
@@ -1836,7 +1894,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>20231026</v>
       </c>
@@ -1850,7 +1908,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>20231027</v>
       </c>
@@ -1864,7 +1922,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>20231027</v>
       </c>
@@ -1878,7 +1936,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>20231027</v>
       </c>
@@ -1892,7 +1950,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>20231028</v>
       </c>
@@ -1906,7 +1964,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>20231028</v>
       </c>
@@ -1920,7 +1978,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>20231028</v>
       </c>
@@ -1934,7 +1992,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>20231028</v>
       </c>
@@ -1948,7 +2006,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>20231028</v>
       </c>
@@ -1962,7 +2020,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>20231028</v>
       </c>
@@ -1976,7 +2034,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>20231028</v>
       </c>
@@ -1990,7 +2048,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>20231028</v>
       </c>
@@ -2004,7 +2062,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>20231028</v>
       </c>
@@ -2018,7 +2076,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>20231028</v>
       </c>
@@ -2032,7 +2090,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>20231028</v>
       </c>
@@ -2046,7 +2104,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>20231028</v>
       </c>
@@ -2059,8 +2117,11 @@
       <c r="E85" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>20231028</v>
       </c>
@@ -2074,7 +2135,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>20231028</v>
       </c>
@@ -2088,7 +2149,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>20231028</v>
       </c>
@@ -2102,7 +2163,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>20231028</v>
       </c>
@@ -2116,7 +2177,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>20231028</v>
       </c>

</xml_diff>